<commit_message>
updated cultural-interest-places with places for commerce, required in the municipal web sites design project (designers). Please see owl:versionInfo metadata for more details
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-culture/cultural-interest-places/cultural-interest-places.xlsx
+++ b/VocabolariControllati/classifications-for-culture/cultural-interest-places/cultural-interest-places.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/Cultural-ON/VocTipoLuoghi/cultural-interest-place/v0.2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Desktop/AGID/NuovoDATIGOV/DAF/Git/OntologieVocabolariControllati/VocabolariControllati/classifications-for-culture/cultural-interest-places/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF08C61B-E414-8348-B18E-9FFB591EC307}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D34380B-2944-3840-88DC-040FE42CD25D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="255">
   <si>
     <t>Architettura militare e fortificata</t>
   </si>
@@ -759,6 +759,42 @@
   </si>
   <si>
     <t>Ghiacciai</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Architettura commerciale</t>
+  </si>
+  <si>
+    <t>Luogo per il commercio</t>
+  </si>
+  <si>
+    <t>Luoghi per il commercio</t>
+  </si>
+  <si>
+    <t>ARCHITETTURA COMMERCIALE</t>
+  </si>
+  <si>
+    <t>Mercato</t>
+  </si>
+  <si>
+    <t>Farmacia</t>
+  </si>
+  <si>
+    <t>Mercati</t>
+  </si>
+  <si>
+    <t>Farmacie</t>
+  </si>
+  <si>
+    <t>Ricomprende i mercati rionali, i mercati comunali, i mercati al coperto</t>
+  </si>
+  <si>
+    <t>L.1</t>
+  </si>
+  <si>
+    <t>L.2</t>
   </si>
 </sst>
 </file>
@@ -1134,10 +1170,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K141"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E56" zoomScale="113" zoomScaleNormal="48" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="113" zoomScaleNormal="48" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1151,10 +1187,10 @@
     <col min="7" max="7" width="41.1640625" customWidth="1"/>
     <col min="8" max="8" width="47" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="80" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="80" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -1182,11 +1218,11 @@
       <c r="I1" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1211,7 +1247,7 @@
       </c>
       <c r="I2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1238,7 +1274,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1265,7 +1301,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
@@ -1292,7 +1328,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -1319,7 +1355,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1344,7 +1380,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1370,11 +1406,11 @@
       <c r="I8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
@@ -1401,7 +1437,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -1428,7 +1464,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
@@ -1455,7 +1491,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -1482,7 +1518,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>7</v>
       </c>
@@ -1507,7 +1543,7 @@
       </c>
       <c r="I13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>7</v>
       </c>
@@ -1534,7 +1570,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>8</v>
       </c>
@@ -1558,9 +1594,9 @@
         <v>181</v>
       </c>
       <c r="I15" s="4"/>
-      <c r="K15" s="6"/>
-    </row>
-    <row r="16" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>8</v>
       </c>
@@ -1584,7 +1620,7 @@
         <v>199</v>
       </c>
       <c r="I16" s="4"/>
-      <c r="K16" s="6"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
@@ -2742,7 +2778,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>133</v>
       </c>
@@ -2762,7 +2798,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>133</v>
       </c>
@@ -2781,11 +2817,11 @@
       <c r="H66" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="K66" s="1" t="s">
+      <c r="J66" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>133</v>
       </c>
@@ -2805,7 +2841,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>133</v>
       </c>
@@ -2825,7 +2861,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>133</v>
       </c>
@@ -2845,7 +2881,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>133</v>
       </c>
@@ -2865,7 +2901,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>133</v>
       </c>
@@ -2885,7 +2921,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>166</v>
       </c>
@@ -2909,31 +2945,78 @@
         <v>236</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A73" s="1"/>
-      <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:11" ht="18" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G73" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="F75" s="1"/>
     </row>
-    <row r="76" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
     </row>
-    <row r="77" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
     </row>
-    <row r="78" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
     </row>
-    <row r="79" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
     </row>
-    <row r="80" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
     </row>
     <row r="81" spans="1:1" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
new version of cultural-interest-places controlled vocabulary. All the changes applied to the controlled voculabulary are clearly identified in the owl:versionInfo property of the vocabulary, in the readme and in comments left within the vocabulary in RDF/turtle. The new version has been required in order to meet specific requirements of people working on the design of municipalities' institutional web sites
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-culture/cultural-interest-places/cultural-interest-places.xlsx
+++ b/VocabolariControllati/classifications-for-culture/cultural-interest-places/cultural-interest-places.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Desktop/AGID/NuovoDATIGOV/DAF/Git/OntologieVocabolariControllati/VocabolariControllati/classifications-for-culture/cultural-interest-places/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7D34380B-2944-3840-88DC-040FE42CD25D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4101BC8-F5A1-604E-9BCC-21318134CFAD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="318">
   <si>
     <t>Architettura militare e fortificata</t>
   </si>
@@ -795,6 +795,195 @@
   </si>
   <si>
     <t>L.2</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Centro per l'assistenza e la tutela sociale</t>
+  </si>
+  <si>
+    <t>Centri per l'assistenza e la tutela sociale</t>
+  </si>
+  <si>
+    <t>ARCHITETTURA OSPEDALIERA, ASSISTENZIALE E PER LA TUTELA SOCIALE</t>
+  </si>
+  <si>
+    <t>M.1</t>
+  </si>
+  <si>
+    <t>Ospizio</t>
+  </si>
+  <si>
+    <t>Casa di riposo</t>
+  </si>
+  <si>
+    <t>Ospizi</t>
+  </si>
+  <si>
+    <t>M.2</t>
+  </si>
+  <si>
+    <t>Centro di accoglienza</t>
+  </si>
+  <si>
+    <t>Centi di accoglienza</t>
+  </si>
+  <si>
+    <t>M.3</t>
+  </si>
+  <si>
+    <t>Ospedale</t>
+  </si>
+  <si>
+    <t>Ospedali</t>
+  </si>
+  <si>
+    <t>I.2</t>
+  </si>
+  <si>
+    <t>Piscina</t>
+  </si>
+  <si>
+    <t>Piscine</t>
+  </si>
+  <si>
+    <t>I.3</t>
+  </si>
+  <si>
+    <t>Stadio</t>
+  </si>
+  <si>
+    <t>I.4</t>
+  </si>
+  <si>
+    <t>Terme</t>
+  </si>
+  <si>
+    <t>I.5</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Infrastruttura e impianto</t>
+  </si>
+  <si>
+    <t>Infrastrutture e impianti</t>
+  </si>
+  <si>
+    <t>N.1</t>
+  </si>
+  <si>
+    <t>Centro di raccolta</t>
+  </si>
+  <si>
+    <t>Centri di raccolta</t>
+  </si>
+  <si>
+    <t>N.2</t>
+  </si>
+  <si>
+    <t>Acquedotto</t>
+  </si>
+  <si>
+    <t>N.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aeroporto </t>
+  </si>
+  <si>
+    <t>Aeroporti</t>
+  </si>
+  <si>
+    <t>Acquedotti</t>
+  </si>
+  <si>
+    <t>N.4</t>
+  </si>
+  <si>
+    <t>Porto</t>
+  </si>
+  <si>
+    <t>Porti</t>
+  </si>
+  <si>
+    <t>Casa da gioco</t>
+  </si>
+  <si>
+    <t>Casinò</t>
+  </si>
+  <si>
+    <t>I.6</t>
+  </si>
+  <si>
+    <t>Circolo sportivo</t>
+  </si>
+  <si>
+    <t>Circoli sportivi</t>
+  </si>
+  <si>
+    <t>Il concetto di palestra potrebbe rientrare in questa voce</t>
+  </si>
+  <si>
+    <t>ARCHITETTURA PER LE INFRASTRUTTURE E IMPIANTI</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>Struttura ricettiva</t>
+  </si>
+  <si>
+    <t>ARCHITETTURA ALBERGHIERA E RICETTIVA</t>
+  </si>
+  <si>
+    <t>Strutture ricettive</t>
+  </si>
+  <si>
+    <t>O.1</t>
+  </si>
+  <si>
+    <t>Albergo</t>
+  </si>
+  <si>
+    <t>Alberghi</t>
+  </si>
+  <si>
+    <t>O.2</t>
+  </si>
+  <si>
+    <t>Foresteria</t>
+  </si>
+  <si>
+    <t>Foresterie</t>
+  </si>
+  <si>
+    <t>O.3</t>
+  </si>
+  <si>
+    <t>Rifugio</t>
+  </si>
+  <si>
+    <t>Rifugi</t>
+  </si>
+  <si>
+    <t>O.4</t>
+  </si>
+  <si>
+    <t>Rifugio per animali</t>
+  </si>
+  <si>
+    <t>Rifugi  per animali</t>
+  </si>
+  <si>
+    <t>I.7</t>
+  </si>
+  <si>
+    <t>Piazza</t>
+  </si>
+  <si>
+    <t>Piazze</t>
   </si>
 </sst>
 </file>
@@ -1170,10 +1359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:J147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" zoomScale="113" zoomScaleNormal="48" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="48" workbookViewId="0">
+      <selection activeCell="A78" sqref="A78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2947,124 +3136,472 @@
     </row>
     <row r="73" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>243</v>
+        <v>166</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>244</v>
+        <v>167</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>245</v>
+        <v>171</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>246</v>
-      </c>
-      <c r="E73" s="4" t="s">
-        <v>247</v>
-      </c>
+        <v>189</v>
+      </c>
+      <c r="E73" s="4"/>
       <c r="F73" s="1" t="s">
-        <v>253</v>
+        <v>269</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>248</v>
+        <v>270</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>252</v>
+        <v>271</v>
       </c>
     </row>
     <row r="74" spans="1:10" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E74" s="4"/>
+      <c r="F74" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="H74" s="4"/>
+    </row>
+    <row r="75" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E75" s="4"/>
+      <c r="F75" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="H75" s="4"/>
+    </row>
+    <row r="76" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E76" s="4"/>
+      <c r="F76" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="G76" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A77" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E77" s="4"/>
+      <c r="F77" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="E78" s="4"/>
+      <c r="F78" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>316</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="J78" s="4"/>
+    </row>
+    <row r="79" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B79" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C79" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="D74" s="4" t="s">
+      <c r="D79" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="E74" s="4" t="s">
+      <c r="E79" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F79" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="G79" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="J79" s="4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="F80" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="G74" s="4" t="s">
+      <c r="G80" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="H74" s="4" t="s">
+      <c r="H80" s="4" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
-      <c r="F75" s="1"/>
-    </row>
-    <row r="76" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A78" s="1"/>
-    </row>
-    <row r="79" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A79" s="1"/>
-    </row>
-    <row r="80" spans="1:10" ht="18" x14ac:dyDescent="0.2">
-      <c r="A80" s="1"/>
-    </row>
-    <row r="81" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A81" s="1"/>
-    </row>
-    <row r="82" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A84" s="1"/>
-    </row>
-    <row r="85" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A85" s="1"/>
-    </row>
-    <row r="86" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A88" s="1"/>
-    </row>
-    <row r="89" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A89" s="1"/>
-    </row>
-    <row r="90" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A90" s="1"/>
-    </row>
-    <row r="91" spans="1:1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A91" s="1"/>
-    </row>
-    <row r="92" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G81" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="H82" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A83" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="G83" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A84" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="G84" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A85" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="G85" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A86" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="G86" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A87" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="G87" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="H87" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A88" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="G88" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A89" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D89" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A90" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F90" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="G90" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A91" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="D91" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
     </row>
-    <row r="93" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
     </row>
-    <row r="94" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
     </row>
-    <row r="95" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
     </row>
-    <row r="96" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
     </row>
     <row r="97" spans="1:1" ht="18" x14ac:dyDescent="0.2">
@@ -3201,6 +3738,24 @@
     </row>
     <row r="141" spans="1:1" ht="18" x14ac:dyDescent="0.2">
       <c r="A141" s="1"/>
+    </row>
+    <row r="142" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A142" s="1"/>
+    </row>
+    <row r="143" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A143" s="1"/>
+    </row>
+    <row r="144" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="145" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A145" s="1"/>
+    </row>
+    <row r="146" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A146" s="1"/>
+    </row>
+    <row r="147" spans="1:1" ht="18" x14ac:dyDescent="0.2">
+      <c r="A147" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>